<commit_message>
[FEAT] Ya funciona todo, solo falta guardar todo en un log
</commit_message>
<xml_diff>
--- a/program/EEPROM_Container_Review_Checkist_GM_iPB_GlobalB_BB95659.xlsx
+++ b/program/EEPROM_Container_Review_Checkist_GM_iPB_GlobalB_BB95659.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcaf9\Documents\Escuela\10mo Semestre\PITE\BOSCH\bosch_eeprom\program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718760D3-88D3-4E91-9CA5-F32B5DB9D035}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DF1510-220A-4C2E-9C54-664EBEE75645}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12744" yWindow="3864" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="77">
   <si>
     <t>E²PROM Container Review Checklist</t>
   </si>
@@ -142,9 +142,6 @@
   </si>
   <si>
     <t>TestData_07</t>
-  </si>
-  <si>
-    <t>12345</t>
   </si>
   <si>
     <t>TestData_08</t>
@@ -271,22 +268,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -307,12 +292,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <name val="Arial"/>
@@ -325,7 +304,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -388,12 +367,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -402,11 +375,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -673,152 +641,146 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
-    <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -1108,11 +1070,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S334"/>
+  <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S24" sqref="S24"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1129,7 +1091,7 @@
     <col min="10" max="10" width="14" style="9" customWidth="1"/>
     <col min="11" max="11" width="12.5546875" style="9" customWidth="1"/>
     <col min="12" max="12" width="16.88671875" style="9" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" style="40" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" style="39" customWidth="1"/>
     <col min="14" max="14" width="21.88671875" style="11" customWidth="1"/>
     <col min="15" max="15" width="46.109375" style="9" customWidth="1"/>
     <col min="16" max="16" width="10.88671875" style="9" customWidth="1"/>
@@ -1158,7 +1120,7 @@
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
-      <c r="M1" s="37"/>
+      <c r="M1" s="36"/>
       <c r="N1" s="10"/>
       <c r="O1" s="6"/>
     </row>
@@ -1177,7 +1139,7 @@
       <c r="J2" s="13"/>
       <c r="K2" s="13"/>
       <c r="L2" s="13"/>
-      <c r="M2" s="38"/>
+      <c r="M2" s="37"/>
       <c r="N2" s="14"/>
       <c r="O2" s="15"/>
     </row>
@@ -1198,7 +1160,7 @@
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
-      <c r="M3" s="38"/>
+      <c r="M3" s="37"/>
       <c r="N3" s="14"/>
       <c r="O3" s="15"/>
     </row>
@@ -1219,7 +1181,7 @@
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
-      <c r="M4" s="38"/>
+      <c r="M4" s="37"/>
       <c r="N4" s="14"/>
       <c r="O4" s="15"/>
       <c r="P4" s="16"/>
@@ -1242,7 +1204,7 @@
       <c r="J5" s="18"/>
       <c r="K5" s="18"/>
       <c r="L5" s="18"/>
-      <c r="M5" s="39"/>
+      <c r="M5" s="38"/>
       <c r="N5" s="19"/>
       <c r="O5" s="20"/>
       <c r="P5" s="21"/>
@@ -1251,102 +1213,102 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
-      <c r="M6" s="55"/>
-      <c r="N6" s="55"/>
-      <c r="O6" s="56"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="52"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="59"/>
-      <c r="K7" s="59"/>
-      <c r="L7" s="59"/>
-      <c r="M7" s="59"/>
-      <c r="N7" s="59"/>
-      <c r="O7" s="60"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="55"/>
+      <c r="M7" s="55"/>
+      <c r="N7" s="55"/>
+      <c r="O7" s="56"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="59"/>
-      <c r="J8" s="59"/>
-      <c r="K8" s="59"/>
-      <c r="L8" s="59"/>
-      <c r="M8" s="59"/>
-      <c r="N8" s="59"/>
-      <c r="O8" s="60"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="55"/>
+      <c r="N8" s="55"/>
+      <c r="O8" s="56"/>
     </row>
     <row r="9" spans="1:19" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="27"/>
-      <c r="D9" s="57" t="s">
+      <c r="D9" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="55"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="43"/>
-      <c r="N9" s="50" t="s">
+      <c r="E9" s="51"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+      <c r="N9" s="46" t="s">
         <v>15</v>
       </c>
       <c r="O9" s="22"/>
     </row>
     <row r="10" spans="1:19" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="41"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="51" t="s">
+      <c r="A10" s="40"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="52"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="64" t="s">
+      <c r="E10" s="48"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="52"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="63" t="s">
+      <c r="H10" s="48"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="52"/>
-      <c r="L10" s="53"/>
-      <c r="N10" s="42"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="49"/>
+      <c r="N10" s="41"/>
       <c r="O10" s="22"/>
     </row>
     <row r="11" spans="1:19" s="11" customFormat="1" ht="52.8" customHeight="1" x14ac:dyDescent="0.25">
@@ -1368,22 +1330,22 @@
       <c r="F11" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="44" t="s">
+      <c r="G11" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="44" t="s">
+      <c r="H11" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="44" t="s">
+      <c r="I11" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="45" t="s">
+      <c r="J11" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="K11" s="45" t="s">
+      <c r="K11" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="L11" s="45" t="s">
+      <c r="L11" s="44" t="s">
         <v>24</v>
       </c>
       <c r="M11" s="32" t="s">
@@ -1410,7 +1372,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="23">
         <v>6</v>
@@ -1437,7 +1399,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="23">
         <v>10</v>
@@ -1464,7 +1426,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="23">
         <v>100</v>
@@ -1489,7 +1451,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" s="23">
         <v>9</v>
@@ -1512,7 +1474,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16" s="23">
         <v>87</v>
@@ -1539,7 +1501,7 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B17" s="23">
         <v>56</v>
@@ -1564,7 +1526,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="23">
         <v>32</v>
@@ -1578,7 +1540,9 @@
       </c>
       <c r="H18" s="24"/>
       <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
+      <c r="J18" s="24" t="s">
+        <v>33</v>
+      </c>
       <c r="K18" s="24"/>
       <c r="L18" s="24"/>
       <c r="M18" s="24" t="s">
@@ -1589,7 +1553,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" s="23">
         <v>78</v>
@@ -1606,7 +1570,9 @@
         <v>33</v>
       </c>
       <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
+      <c r="K19" s="24" t="s">
+        <v>33</v>
+      </c>
       <c r="L19" s="24"/>
       <c r="M19" s="24" t="s">
         <v>35</v>
@@ -1618,11 +1584,11 @@
       <c r="A20" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="23" t="s">
-        <v>37</v>
+      <c r="B20" s="23">
+        <v>123456</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="24"/>
@@ -1638,7 +1604,9 @@
       <c r="I20" s="24"/>
       <c r="J20" s="24"/>
       <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
+      <c r="L20" s="24" t="s">
+        <v>33</v>
+      </c>
       <c r="M20" s="24" t="s">
         <v>35</v>
       </c>
@@ -1650,13 +1618,13 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="23" t="s">
-        <v>39</v>
-      </c>
       <c r="C21" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D21" s="24"/>
       <c r="E21" s="24" t="s">
@@ -1676,13 +1644,13 @@
       </c>
       <c r="N21" s="25"/>
       <c r="O21" s="35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P21" s="9">
         <v>7</v>
       </c>
       <c r="Q21" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R21" s="9">
         <v>8</v>
@@ -1693,13 +1661,13 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="23" t="s">
-        <v>41</v>
-      </c>
       <c r="C22" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D22" s="24"/>
       <c r="E22" s="24" t="s">
@@ -1720,16 +1688,16 @@
         <v>35</v>
       </c>
       <c r="N22" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O22" s="35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P22" s="9">
         <v>6</v>
       </c>
       <c r="Q22" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R22" s="9">
         <v>7</v>
@@ -1740,13 +1708,13 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="23" t="s">
-        <v>43</v>
-      </c>
       <c r="C23" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D23" s="24" t="s">
         <v>33</v>
@@ -1771,16 +1739,16 @@
         <v>35</v>
       </c>
       <c r="N23" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O23" s="35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P23" s="9">
         <v>5</v>
       </c>
       <c r="Q23" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R23" s="9">
         <v>6</v>
@@ -1791,13 +1759,13 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="23" t="s">
-        <v>45</v>
-      </c>
       <c r="C24" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D24" s="24" t="s">
         <v>33</v>
@@ -1817,17 +1785,17 @@
       <c r="K24" s="24"/>
       <c r="L24" s="24"/>
       <c r="M24" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N24" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O24" s="35"/>
       <c r="P24" s="9">
         <v>10</v>
       </c>
       <c r="Q24" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R24" s="9">
         <v>5</v>
@@ -1838,13 +1806,13 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="23" t="s">
-        <v>45</v>
-      </c>
       <c r="C25" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D25" s="24"/>
       <c r="E25" s="24" t="s">
@@ -1860,19 +1828,19 @@
       <c r="K25" s="24"/>
       <c r="L25" s="24"/>
       <c r="M25" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="N25" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="N25" s="25" t="s">
-        <v>65</v>
-      </c>
       <c r="O25" s="35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P25" s="9">
         <v>6</v>
       </c>
       <c r="Q25" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R25" s="9">
         <v>4</v>
@@ -1881,1116 +1849,6 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="23"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="24"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="25"/>
-      <c r="O26" s="35"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B27" s="23"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="24"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="25"/>
-      <c r="O27" s="35"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B28" s="23"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="25"/>
-      <c r="O28" s="35"/>
-    </row>
-    <row r="29" spans="1:19" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="23"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="24"/>
-      <c r="K29" s="24"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="24"/>
-      <c r="N29" s="25"/>
-      <c r="O29" s="35"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B30" s="23"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="24"/>
-      <c r="M30" s="24"/>
-      <c r="N30" s="25"/>
-      <c r="O30" s="35"/>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B31" s="23"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="25"/>
-      <c r="O31" s="35"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="23"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="24"/>
-      <c r="J32" s="24"/>
-      <c r="K32" s="24"/>
-      <c r="L32" s="24"/>
-      <c r="M32" s="24"/>
-      <c r="N32" s="25"/>
-      <c r="O32" s="35"/>
-    </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="23"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="24"/>
-      <c r="K33" s="24"/>
-      <c r="L33" s="24"/>
-      <c r="M33" s="24"/>
-      <c r="N33" s="25"/>
-      <c r="O33" s="35"/>
-    </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B34" s="23"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="24"/>
-      <c r="K34" s="24"/>
-      <c r="L34" s="24"/>
-      <c r="M34" s="24"/>
-      <c r="N34" s="25"/>
-      <c r="O34" s="35"/>
-    </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="23"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="24"/>
-      <c r="J35" s="24"/>
-      <c r="K35" s="24"/>
-      <c r="L35" s="24"/>
-      <c r="M35" s="24"/>
-      <c r="N35" s="25"/>
-      <c r="O35" s="35"/>
-    </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="23"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24"/>
-      <c r="I36" s="24"/>
-      <c r="J36" s="24"/>
-      <c r="K36" s="24"/>
-      <c r="L36" s="24"/>
-      <c r="M36" s="24"/>
-      <c r="N36" s="25"/>
-      <c r="O36" s="35"/>
-    </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B37" s="23"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="24"/>
-      <c r="J37" s="24"/>
-      <c r="K37" s="24"/>
-      <c r="L37" s="24"/>
-      <c r="M37" s="24"/>
-      <c r="N37" s="25"/>
-      <c r="O37" s="35"/>
-    </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B38" s="23"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="24"/>
-      <c r="J38" s="24"/>
-      <c r="K38" s="24"/>
-      <c r="L38" s="24"/>
-      <c r="M38" s="24"/>
-      <c r="N38" s="25"/>
-      <c r="O38" s="35"/>
-    </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B39" s="23"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="24"/>
-      <c r="J39" s="24"/>
-      <c r="K39" s="24"/>
-      <c r="L39" s="24"/>
-      <c r="M39" s="24"/>
-      <c r="N39" s="25"/>
-      <c r="O39" s="35"/>
-    </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B40" s="23"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="24"/>
-      <c r="I40" s="24"/>
-      <c r="J40" s="24"/>
-      <c r="K40" s="24"/>
-      <c r="L40" s="24"/>
-      <c r="M40" s="24"/>
-      <c r="N40" s="25"/>
-      <c r="O40" s="35"/>
-    </row>
-    <row r="41" spans="2:15" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="23"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="24"/>
-      <c r="G41" s="24"/>
-      <c r="H41" s="24"/>
-      <c r="I41" s="24"/>
-      <c r="J41" s="24"/>
-      <c r="K41" s="24"/>
-      <c r="L41" s="24"/>
-      <c r="M41" s="24"/>
-      <c r="N41" s="25"/>
-      <c r="O41" s="35"/>
-    </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="23"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24"/>
-      <c r="G42" s="24"/>
-      <c r="H42" s="24"/>
-      <c r="I42" s="24"/>
-      <c r="J42" s="24"/>
-      <c r="K42" s="24"/>
-      <c r="L42" s="24"/>
-      <c r="M42" s="24"/>
-      <c r="N42" s="25"/>
-      <c r="O42" s="35"/>
-    </row>
-    <row r="43" spans="2:15" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="23"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24"/>
-      <c r="G43" s="24"/>
-      <c r="H43" s="24"/>
-      <c r="I43" s="24"/>
-      <c r="J43" s="24"/>
-      <c r="K43" s="24"/>
-      <c r="L43" s="24"/>
-      <c r="M43" s="24"/>
-      <c r="N43" s="25"/>
-      <c r="O43" s="35"/>
-    </row>
-    <row r="44" spans="2:15" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="23"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="24"/>
-      <c r="H44" s="24"/>
-      <c r="I44" s="24"/>
-      <c r="J44" s="24"/>
-      <c r="K44" s="24"/>
-      <c r="L44" s="24"/>
-      <c r="M44" s="24"/>
-      <c r="N44" s="25"/>
-      <c r="O44" s="35"/>
-    </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B45" s="23"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="24"/>
-      <c r="H45" s="24"/>
-      <c r="I45" s="24"/>
-      <c r="J45" s="24"/>
-      <c r="K45" s="24"/>
-      <c r="L45" s="24"/>
-      <c r="M45" s="24"/>
-      <c r="N45" s="25"/>
-      <c r="O45" s="35"/>
-    </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="23"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="24"/>
-      <c r="F46" s="24"/>
-      <c r="G46" s="24"/>
-      <c r="H46" s="24"/>
-      <c r="I46" s="24"/>
-      <c r="J46" s="24"/>
-      <c r="K46" s="24"/>
-      <c r="L46" s="24"/>
-      <c r="M46" s="24"/>
-      <c r="N46" s="25"/>
-      <c r="O46" s="35"/>
-    </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B47" s="23"/>
-      <c r="C47" s="24"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="24"/>
-      <c r="G47" s="24"/>
-      <c r="H47" s="24"/>
-      <c r="I47" s="24"/>
-      <c r="J47" s="24"/>
-      <c r="K47" s="24"/>
-      <c r="L47" s="24"/>
-      <c r="M47" s="24"/>
-      <c r="N47" s="25"/>
-      <c r="O47" s="35"/>
-    </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B48" s="23"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="24"/>
-      <c r="H48" s="24"/>
-      <c r="I48" s="24"/>
-      <c r="J48" s="24"/>
-      <c r="K48" s="24"/>
-      <c r="L48" s="24"/>
-      <c r="M48" s="24"/>
-      <c r="N48" s="25"/>
-      <c r="O48" s="35"/>
-    </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B49" s="23"/>
-      <c r="C49" s="24"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="24"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="24"/>
-      <c r="H49" s="24"/>
-      <c r="I49" s="24"/>
-      <c r="J49" s="24"/>
-      <c r="K49" s="24"/>
-      <c r="L49" s="24"/>
-      <c r="M49" s="24"/>
-      <c r="N49" s="25"/>
-      <c r="O49" s="35"/>
-    </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B50" s="23"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24"/>
-      <c r="G50" s="24"/>
-      <c r="H50" s="24"/>
-      <c r="I50" s="24"/>
-      <c r="J50" s="24"/>
-      <c r="K50" s="24"/>
-      <c r="L50" s="24"/>
-      <c r="M50" s="24"/>
-      <c r="N50" s="25"/>
-      <c r="O50" s="35"/>
-    </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B51" s="23"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="24"/>
-      <c r="G51" s="24"/>
-      <c r="H51" s="24"/>
-      <c r="I51" s="24"/>
-      <c r="J51" s="24"/>
-      <c r="K51" s="24"/>
-      <c r="L51" s="24"/>
-      <c r="M51" s="24"/>
-      <c r="N51" s="25"/>
-      <c r="O51" s="35"/>
-    </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B52" s="23"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="24"/>
-      <c r="H52" s="24"/>
-      <c r="I52" s="24"/>
-      <c r="J52" s="24"/>
-      <c r="K52" s="24"/>
-      <c r="L52" s="24"/>
-      <c r="M52" s="24"/>
-      <c r="N52" s="25"/>
-      <c r="O52" s="35"/>
-    </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B53" s="23"/>
-      <c r="C53" s="24"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="24"/>
-      <c r="F53" s="24"/>
-      <c r="G53" s="24"/>
-      <c r="H53" s="24"/>
-      <c r="I53" s="24"/>
-      <c r="J53" s="24"/>
-      <c r="K53" s="24"/>
-      <c r="L53" s="24"/>
-      <c r="M53" s="24"/>
-      <c r="N53" s="25"/>
-      <c r="O53" s="35"/>
-    </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B54" s="23"/>
-      <c r="C54" s="24"/>
-      <c r="D54" s="24"/>
-      <c r="E54" s="24"/>
-      <c r="F54" s="24"/>
-      <c r="G54" s="24"/>
-      <c r="H54" s="24"/>
-      <c r="I54" s="24"/>
-      <c r="J54" s="24"/>
-      <c r="K54" s="24"/>
-      <c r="L54" s="24"/>
-      <c r="M54" s="24"/>
-      <c r="N54" s="25"/>
-      <c r="O54" s="35"/>
-    </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B55" s="23"/>
-      <c r="C55" s="24"/>
-      <c r="D55" s="24"/>
-      <c r="E55" s="24"/>
-      <c r="F55" s="24"/>
-      <c r="G55" s="24"/>
-      <c r="H55" s="24"/>
-      <c r="I55" s="24"/>
-      <c r="J55" s="24"/>
-      <c r="K55" s="24"/>
-      <c r="L55" s="24"/>
-      <c r="M55" s="24"/>
-      <c r="N55" s="25"/>
-      <c r="O55" s="35"/>
-    </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B56" s="23"/>
-      <c r="C56" s="24"/>
-      <c r="D56" s="24"/>
-      <c r="E56" s="24"/>
-      <c r="F56" s="24"/>
-      <c r="G56" s="24"/>
-      <c r="H56" s="24"/>
-      <c r="I56" s="24"/>
-      <c r="J56" s="24"/>
-      <c r="K56" s="24"/>
-      <c r="L56" s="24"/>
-      <c r="M56" s="24"/>
-      <c r="N56" s="25"/>
-      <c r="O56" s="35"/>
-    </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="23"/>
-      <c r="C57" s="24"/>
-      <c r="D57" s="24"/>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24"/>
-      <c r="G57" s="24"/>
-      <c r="H57" s="24"/>
-      <c r="I57" s="24"/>
-      <c r="J57" s="24"/>
-      <c r="K57" s="24"/>
-      <c r="L57" s="24"/>
-      <c r="M57" s="24"/>
-      <c r="N57" s="25"/>
-      <c r="O57" s="35"/>
-    </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B58" s="23"/>
-      <c r="C58" s="24"/>
-      <c r="D58" s="24"/>
-      <c r="E58" s="24"/>
-      <c r="F58" s="24"/>
-      <c r="G58" s="24"/>
-      <c r="H58" s="24"/>
-      <c r="I58" s="24"/>
-      <c r="J58" s="24"/>
-      <c r="K58" s="24"/>
-      <c r="L58" s="24"/>
-      <c r="M58" s="24"/>
-      <c r="N58" s="25"/>
-      <c r="O58" s="35"/>
-    </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B59" s="23"/>
-      <c r="C59" s="24"/>
-      <c r="D59" s="24"/>
-      <c r="E59" s="24"/>
-      <c r="F59" s="24"/>
-      <c r="G59" s="24"/>
-      <c r="H59" s="24"/>
-      <c r="I59" s="24"/>
-      <c r="J59" s="24"/>
-      <c r="K59" s="24"/>
-      <c r="L59" s="24"/>
-      <c r="M59" s="24"/>
-      <c r="N59" s="25"/>
-      <c r="O59" s="35"/>
-    </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B60" s="23"/>
-      <c r="C60" s="24"/>
-      <c r="D60" s="24"/>
-      <c r="E60" s="24"/>
-      <c r="F60" s="24"/>
-      <c r="G60" s="24"/>
-      <c r="H60" s="24"/>
-      <c r="I60" s="24"/>
-      <c r="J60" s="24"/>
-      <c r="K60" s="24"/>
-      <c r="L60" s="24"/>
-      <c r="M60" s="24"/>
-      <c r="N60" s="25"/>
-      <c r="O60" s="35"/>
-    </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B61" s="23"/>
-      <c r="C61" s="24"/>
-      <c r="D61" s="24"/>
-      <c r="E61" s="24"/>
-      <c r="F61" s="24"/>
-      <c r="G61" s="24"/>
-      <c r="H61" s="24"/>
-      <c r="I61" s="24"/>
-      <c r="J61" s="24"/>
-      <c r="K61" s="24"/>
-      <c r="L61" s="24"/>
-      <c r="M61" s="24"/>
-      <c r="N61" s="25"/>
-      <c r="O61" s="35"/>
-    </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B62" s="23"/>
-      <c r="C62" s="24"/>
-      <c r="D62" s="24"/>
-      <c r="E62" s="24"/>
-      <c r="F62" s="24"/>
-      <c r="G62" s="24"/>
-      <c r="H62" s="24"/>
-      <c r="I62" s="24"/>
-      <c r="J62" s="24"/>
-      <c r="K62" s="24"/>
-      <c r="L62" s="24"/>
-      <c r="M62" s="24"/>
-      <c r="N62" s="25"/>
-      <c r="O62" s="35"/>
-    </row>
-    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B63" s="23"/>
-      <c r="C63" s="24"/>
-      <c r="D63" s="24"/>
-      <c r="E63" s="24"/>
-      <c r="F63" s="24"/>
-      <c r="G63" s="24"/>
-      <c r="H63" s="24"/>
-      <c r="I63" s="24"/>
-      <c r="J63" s="24"/>
-      <c r="K63" s="24"/>
-      <c r="L63" s="24"/>
-      <c r="M63" s="24"/>
-      <c r="N63" s="25"/>
-      <c r="O63" s="35"/>
-    </row>
-    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B64" s="23"/>
-      <c r="C64" s="24"/>
-      <c r="D64" s="24"/>
-      <c r="E64" s="24"/>
-      <c r="F64" s="24"/>
-      <c r="G64" s="24"/>
-      <c r="H64" s="24"/>
-      <c r="I64" s="24"/>
-      <c r="J64" s="24"/>
-      <c r="K64" s="24"/>
-      <c r="L64" s="24"/>
-      <c r="M64" s="24"/>
-      <c r="N64" s="25"/>
-      <c r="O64" s="35"/>
-    </row>
-    <row r="65" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B65" s="23"/>
-      <c r="C65" s="24"/>
-      <c r="D65" s="24"/>
-      <c r="E65" s="24"/>
-      <c r="F65" s="24"/>
-      <c r="G65" s="24"/>
-      <c r="H65" s="24"/>
-      <c r="I65" s="24"/>
-      <c r="J65" s="24"/>
-      <c r="K65" s="24"/>
-      <c r="L65" s="24"/>
-      <c r="M65" s="24"/>
-      <c r="N65" s="25"/>
-      <c r="O65" s="35"/>
-    </row>
-    <row r="66" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B66" s="23"/>
-      <c r="C66" s="24"/>
-      <c r="D66" s="24"/>
-      <c r="E66" s="24"/>
-      <c r="F66" s="24"/>
-      <c r="G66" s="24"/>
-      <c r="H66" s="24"/>
-      <c r="I66" s="24"/>
-      <c r="J66" s="24"/>
-      <c r="K66" s="24"/>
-      <c r="L66" s="24"/>
-      <c r="M66" s="24"/>
-      <c r="N66" s="25"/>
-      <c r="O66" s="35"/>
-    </row>
-    <row r="67" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B67" s="23"/>
-      <c r="C67" s="24"/>
-      <c r="D67" s="24"/>
-      <c r="E67" s="24"/>
-      <c r="F67" s="24"/>
-      <c r="G67" s="24"/>
-      <c r="H67" s="24"/>
-      <c r="I67" s="24"/>
-      <c r="J67" s="24"/>
-      <c r="K67" s="24"/>
-      <c r="L67" s="24"/>
-      <c r="M67" s="24"/>
-      <c r="N67" s="25"/>
-      <c r="O67" s="35"/>
-    </row>
-    <row r="68" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B68" s="23"/>
-      <c r="C68" s="24"/>
-      <c r="D68" s="24"/>
-      <c r="E68" s="24"/>
-      <c r="F68" s="24"/>
-      <c r="G68" s="24"/>
-      <c r="H68" s="24"/>
-      <c r="I68" s="24"/>
-      <c r="J68" s="24"/>
-      <c r="K68" s="24"/>
-      <c r="L68" s="24"/>
-      <c r="M68" s="24"/>
-      <c r="N68" s="25"/>
-      <c r="O68" s="35"/>
-    </row>
-    <row r="69" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B69" s="23"/>
-      <c r="C69" s="24"/>
-      <c r="D69" s="24"/>
-      <c r="E69" s="24"/>
-      <c r="F69" s="24"/>
-      <c r="G69" s="24"/>
-      <c r="H69" s="24"/>
-      <c r="I69" s="24"/>
-      <c r="J69" s="24"/>
-      <c r="K69" s="24"/>
-      <c r="L69" s="24"/>
-      <c r="M69" s="24"/>
-      <c r="N69" s="25"/>
-      <c r="O69" s="35"/>
-    </row>
-    <row r="70" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B70" s="23"/>
-      <c r="C70" s="24"/>
-      <c r="D70" s="24"/>
-      <c r="E70" s="24"/>
-      <c r="F70" s="24"/>
-      <c r="G70" s="24"/>
-      <c r="H70" s="24"/>
-      <c r="I70" s="24"/>
-      <c r="J70" s="24"/>
-      <c r="K70" s="24"/>
-      <c r="L70" s="24"/>
-      <c r="M70" s="24"/>
-      <c r="N70" s="25"/>
-      <c r="O70" s="35"/>
-    </row>
-    <row r="71" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B71" s="23"/>
-      <c r="C71" s="24"/>
-      <c r="D71" s="24"/>
-      <c r="E71" s="24"/>
-      <c r="F71" s="24"/>
-      <c r="G71" s="24"/>
-      <c r="H71" s="24"/>
-      <c r="I71" s="24"/>
-      <c r="J71" s="24"/>
-      <c r="K71" s="24"/>
-      <c r="L71" s="24"/>
-      <c r="M71" s="24"/>
-      <c r="N71" s="25"/>
-      <c r="O71" s="35"/>
-    </row>
-    <row r="72" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B72" s="23"/>
-      <c r="C72" s="24"/>
-      <c r="D72" s="24"/>
-      <c r="E72" s="24"/>
-      <c r="F72" s="24"/>
-      <c r="G72" s="24"/>
-      <c r="H72" s="24"/>
-      <c r="I72" s="24"/>
-      <c r="J72" s="24"/>
-      <c r="K72" s="24"/>
-      <c r="L72" s="24"/>
-      <c r="M72" s="24"/>
-      <c r="N72" s="25"/>
-      <c r="O72" s="35"/>
-    </row>
-    <row r="73" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B73" s="23"/>
-      <c r="C73" s="24"/>
-      <c r="D73" s="24"/>
-      <c r="E73" s="24"/>
-      <c r="F73" s="24"/>
-      <c r="G73" s="24"/>
-      <c r="H73" s="24"/>
-      <c r="I73" s="24"/>
-      <c r="J73" s="24"/>
-      <c r="K73" s="24"/>
-      <c r="L73" s="24"/>
-      <c r="M73" s="24"/>
-      <c r="N73" s="25"/>
-      <c r="O73" s="35"/>
-    </row>
-    <row r="74" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B74" s="23"/>
-      <c r="C74" s="24"/>
-      <c r="D74" s="24"/>
-      <c r="E74" s="24"/>
-      <c r="F74" s="24"/>
-      <c r="G74" s="24"/>
-      <c r="H74" s="24"/>
-      <c r="I74" s="24"/>
-      <c r="J74" s="24"/>
-      <c r="K74" s="24"/>
-      <c r="L74" s="24"/>
-      <c r="M74" s="24"/>
-      <c r="N74" s="25"/>
-      <c r="O74" s="35"/>
-    </row>
-    <row r="75" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B75" s="23"/>
-      <c r="C75" s="24"/>
-      <c r="D75" s="24"/>
-      <c r="E75" s="24"/>
-      <c r="F75" s="24"/>
-      <c r="G75" s="24"/>
-      <c r="H75" s="24"/>
-      <c r="I75" s="24"/>
-      <c r="J75" s="24"/>
-      <c r="K75" s="24"/>
-      <c r="L75" s="24"/>
-      <c r="M75" s="24"/>
-      <c r="N75" s="25"/>
-      <c r="O75" s="35"/>
-    </row>
-    <row r="76" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B76" s="23"/>
-      <c r="C76" s="24"/>
-      <c r="D76" s="24"/>
-      <c r="E76" s="24"/>
-      <c r="F76" s="24"/>
-      <c r="G76" s="24"/>
-      <c r="H76" s="24"/>
-      <c r="I76" s="24"/>
-      <c r="J76" s="24"/>
-      <c r="K76" s="24"/>
-      <c r="L76" s="24"/>
-      <c r="M76" s="24"/>
-      <c r="N76" s="25"/>
-      <c r="O76" s="35"/>
-    </row>
-    <row r="77" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B77" s="23"/>
-      <c r="C77" s="24"/>
-      <c r="D77" s="24"/>
-      <c r="E77" s="24"/>
-      <c r="F77" s="24"/>
-      <c r="G77" s="24"/>
-      <c r="H77" s="24"/>
-      <c r="I77" s="24"/>
-      <c r="J77" s="24"/>
-      <c r="K77" s="24"/>
-      <c r="L77" s="24"/>
-      <c r="M77" s="24"/>
-      <c r="N77" s="25"/>
-      <c r="O77" s="35"/>
-    </row>
-    <row r="78" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B78" s="23"/>
-      <c r="C78" s="24"/>
-      <c r="D78" s="24"/>
-      <c r="E78" s="24"/>
-      <c r="F78" s="24"/>
-      <c r="G78" s="24"/>
-      <c r="H78" s="24"/>
-      <c r="I78" s="24"/>
-      <c r="J78" s="24"/>
-      <c r="K78" s="24"/>
-      <c r="L78" s="24"/>
-      <c r="M78" s="24"/>
-      <c r="N78" s="25"/>
-      <c r="O78" s="35"/>
-    </row>
-    <row r="79" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B79" s="23"/>
-      <c r="C79" s="24"/>
-      <c r="D79" s="24"/>
-      <c r="E79" s="24"/>
-      <c r="F79" s="24"/>
-      <c r="G79" s="24"/>
-      <c r="H79" s="24"/>
-      <c r="I79" s="24"/>
-      <c r="J79" s="24"/>
-      <c r="K79" s="24"/>
-      <c r="L79" s="24"/>
-      <c r="M79" s="24"/>
-      <c r="N79" s="25"/>
-      <c r="O79" s="35"/>
-    </row>
-    <row r="80" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B80" s="23"/>
-      <c r="C80" s="24"/>
-      <c r="D80" s="24"/>
-      <c r="E80" s="24"/>
-      <c r="F80" s="24"/>
-      <c r="G80" s="24"/>
-      <c r="H80" s="24"/>
-      <c r="I80" s="24"/>
-      <c r="J80" s="24"/>
-      <c r="K80" s="24"/>
-      <c r="L80" s="24"/>
-      <c r="M80" s="24"/>
-      <c r="N80" s="25"/>
-      <c r="O80" s="35"/>
-    </row>
-    <row r="81" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B81" s="23"/>
-      <c r="C81" s="24"/>
-      <c r="D81" s="24"/>
-      <c r="E81" s="24"/>
-      <c r="F81" s="24"/>
-      <c r="G81" s="24"/>
-      <c r="H81" s="24"/>
-      <c r="I81" s="24"/>
-      <c r="J81" s="24"/>
-      <c r="K81" s="24"/>
-      <c r="L81" s="24"/>
-      <c r="M81" s="24"/>
-      <c r="N81" s="25"/>
-      <c r="O81" s="35"/>
-    </row>
-    <row r="82" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B82" s="23"/>
-      <c r="C82" s="24"/>
-      <c r="D82" s="24"/>
-      <c r="E82" s="24"/>
-      <c r="F82" s="24"/>
-      <c r="G82" s="24"/>
-      <c r="H82" s="24"/>
-      <c r="I82" s="24"/>
-      <c r="J82" s="24"/>
-      <c r="K82" s="24"/>
-      <c r="L82" s="24"/>
-      <c r="M82" s="24"/>
-      <c r="N82" s="25"/>
-      <c r="O82" s="35"/>
-    </row>
-    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B83" s="23"/>
-      <c r="C83" s="24"/>
-      <c r="D83" s="24"/>
-      <c r="E83" s="24"/>
-      <c r="F83" s="24"/>
-      <c r="G83" s="24"/>
-      <c r="H83" s="24"/>
-      <c r="I83" s="24"/>
-      <c r="J83" s="24"/>
-      <c r="K83" s="24"/>
-      <c r="L83" s="24"/>
-      <c r="M83" s="24"/>
-      <c r="N83" s="25"/>
-      <c r="O83" s="35"/>
-    </row>
-    <row r="84" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B84" s="23"/>
-      <c r="C84" s="24"/>
-      <c r="D84" s="24"/>
-      <c r="E84" s="24"/>
-      <c r="F84" s="24"/>
-      <c r="G84" s="24"/>
-      <c r="H84" s="24"/>
-      <c r="I84" s="24"/>
-      <c r="J84" s="24"/>
-      <c r="K84" s="24"/>
-      <c r="L84" s="24"/>
-      <c r="M84" s="24"/>
-      <c r="N84" s="25"/>
-      <c r="O84" s="35"/>
-    </row>
-    <row r="85" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B85" s="23"/>
-      <c r="C85" s="24"/>
-      <c r="D85" s="24"/>
-      <c r="E85" s="24"/>
-      <c r="F85" s="24"/>
-      <c r="G85" s="24"/>
-      <c r="H85" s="24"/>
-      <c r="I85" s="24"/>
-      <c r="J85" s="24"/>
-      <c r="K85" s="24"/>
-      <c r="L85" s="24"/>
-      <c r="M85" s="24"/>
-      <c r="N85" s="25"/>
-      <c r="O85" s="35"/>
-    </row>
-    <row r="86" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B86" s="23"/>
-      <c r="C86" s="24"/>
-      <c r="D86" s="24"/>
-      <c r="E86" s="24"/>
-      <c r="F86" s="24"/>
-      <c r="G86" s="24"/>
-      <c r="H86" s="24"/>
-      <c r="I86" s="24"/>
-      <c r="J86" s="24"/>
-      <c r="K86" s="24"/>
-      <c r="L86" s="24"/>
-      <c r="M86" s="24"/>
-      <c r="N86" s="25"/>
-      <c r="O86" s="35"/>
-    </row>
-    <row r="87" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B87" s="23"/>
-      <c r="C87" s="24"/>
-      <c r="D87" s="24"/>
-      <c r="E87" s="24"/>
-      <c r="F87" s="24"/>
-      <c r="G87" s="24"/>
-      <c r="H87" s="24"/>
-      <c r="I87" s="24"/>
-      <c r="J87" s="24"/>
-      <c r="K87" s="24"/>
-      <c r="L87" s="24"/>
-      <c r="M87" s="24"/>
-      <c r="N87" s="25"/>
-      <c r="O87" s="35"/>
-    </row>
-    <row r="88" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B88" s="23"/>
-      <c r="C88" s="24"/>
-      <c r="D88" s="24"/>
-      <c r="E88" s="24"/>
-      <c r="F88" s="24"/>
-      <c r="G88" s="24"/>
-      <c r="H88" s="24"/>
-      <c r="I88" s="24"/>
-      <c r="J88" s="24"/>
-      <c r="K88" s="24"/>
-      <c r="L88" s="24"/>
-      <c r="M88" s="24"/>
-      <c r="N88" s="25"/>
-      <c r="O88" s="35"/>
-    </row>
-    <row r="89" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B89" s="23"/>
-      <c r="C89" s="24"/>
-      <c r="D89" s="24"/>
-      <c r="E89" s="24"/>
-      <c r="F89" s="24"/>
-      <c r="G89" s="24"/>
-      <c r="H89" s="24"/>
-      <c r="I89" s="24"/>
-      <c r="J89" s="24"/>
-      <c r="K89" s="24"/>
-      <c r="L89" s="24"/>
-      <c r="M89" s="24"/>
-      <c r="N89" s="25"/>
-      <c r="O89" s="35"/>
-    </row>
-    <row r="90" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B90" s="23"/>
-      <c r="C90" s="24"/>
-      <c r="D90" s="24"/>
-      <c r="E90" s="24"/>
-      <c r="F90" s="24"/>
-      <c r="G90" s="24"/>
-      <c r="H90" s="24"/>
-      <c r="I90" s="24"/>
-      <c r="J90" s="24"/>
-      <c r="K90" s="24"/>
-      <c r="L90" s="24"/>
-      <c r="M90" s="24"/>
-      <c r="N90" s="25"/>
-      <c r="O90" s="35"/>
-    </row>
-    <row r="91" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B91" s="23"/>
-      <c r="C91" s="24"/>
-      <c r="D91" s="24"/>
-      <c r="E91" s="24"/>
-      <c r="F91" s="24"/>
-      <c r="G91" s="24"/>
-      <c r="H91" s="24"/>
-      <c r="I91" s="24"/>
-      <c r="J91" s="24"/>
-      <c r="K91" s="24"/>
-      <c r="L91" s="24"/>
-      <c r="M91" s="24"/>
-      <c r="N91" s="25"/>
-      <c r="O91" s="35"/>
-    </row>
-    <row r="92" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B92" s="23"/>
-      <c r="C92" s="24"/>
-      <c r="D92" s="24"/>
-      <c r="E92" s="24"/>
-      <c r="F92" s="24"/>
-      <c r="G92" s="24"/>
-      <c r="H92" s="24"/>
-      <c r="I92" s="24"/>
-      <c r="J92" s="24"/>
-      <c r="K92" s="24"/>
-      <c r="L92" s="24"/>
-      <c r="M92" s="24"/>
-      <c r="N92" s="25"/>
-      <c r="O92" s="35"/>
-    </row>
-    <row r="144" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="145" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="146" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="224" ht="39.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="266" spans="1:19" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A266" s="9"/>
-      <c r="B266" s="9"/>
-      <c r="C266" s="9"/>
-      <c r="D266" s="9"/>
-      <c r="E266" s="9"/>
-      <c r="F266" s="9"/>
-      <c r="G266" s="9"/>
-      <c r="H266" s="9"/>
-      <c r="I266" s="9"/>
-      <c r="J266" s="9"/>
-      <c r="K266" s="9"/>
-      <c r="L266" s="9"/>
-      <c r="M266" s="40"/>
-      <c r="N266" s="11"/>
-      <c r="O266" s="9"/>
-      <c r="P266" s="9"/>
-      <c r="Q266" s="9"/>
-      <c r="R266" s="9"/>
-      <c r="S266" s="11"/>
-    </row>
-    <row r="272" spans="1:19" s="47" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="273" s="47" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="274" s="47" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="275" s="47" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="276" s="47" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="277" s="47" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="278" s="47" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="279" s="47" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="280" s="47" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="281" s="47" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="282" s="47" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="328" s="47" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="334" s="47" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A11:S11" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="8">
@@ -3003,18 +1861,18 @@
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="G10:I10"/>
   </mergeCells>
-  <conditionalFormatting sqref="N12:N108">
+  <conditionalFormatting sqref="N12:N25">
     <cfRule type="expression" dxfId="0" priority="201" stopIfTrue="1">
       <formula>AND(NOT(ISBLANK(N12)),M12="range")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="M12:M108" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="M12:M25" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"range,datablock"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0" right="0" top="0.78740157480314965" bottom="0.59055118110236227" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="10" orientation="landscape"/>
+  <pageSetup paperSize="9" scale="10" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;LRobert Bosch GmbH
 &amp;CEEPROM Container Review Checklist&amp;R&amp;D</oddHeader>
@@ -3044,16 +1902,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[CHORE-FIX] Carpetas y archivos eliminados. BBNumber del reporte previo acomodado acorde a su version
</commit_message>
<xml_diff>
--- a/program/EEPROM_Container_Review_Checkist_GM_iPB_GlobalB_BB95659.xlsx
+++ b/program/EEPROM_Container_Review_Checkist_GM_iPB_GlobalB_BB95659.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcaf9\Documents\Escuela\10mo Semestre\PITE\BOSCH\bosch_eeprom\program\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Barajas\Documents\bosch_eeprom\program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DF1510-220A-4C2E-9C54-664EBEE75645}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FF5B74-DA5D-4B87-A0D0-749A2CD6E866}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
     <t>BB-Number</t>
   </si>
   <si>
-    <t>BB95650</t>
-  </si>
-  <si>
     <t>SW-Version</t>
   </si>
   <si>
@@ -262,6 +259,9 @@
   </si>
   <si>
     <t>OSCAR</t>
+  </si>
+  <si>
+    <t>BB95659</t>
   </si>
 </sst>
 </file>
@@ -1074,36 +1074,36 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.6640625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="43.7109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="9" customWidth="1"/>
     <col min="3" max="3" width="14" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="7.109375" style="9" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="9" customWidth="1"/>
     <col min="7" max="7" width="17" style="9" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" style="9" customWidth="1"/>
     <col min="9" max="9" width="19" style="9" customWidth="1"/>
     <col min="10" max="10" width="14" style="9" customWidth="1"/>
-    <col min="11" max="11" width="12.5546875" style="9" customWidth="1"/>
-    <col min="12" max="12" width="16.88671875" style="9" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" style="39" customWidth="1"/>
-    <col min="14" max="14" width="21.88671875" style="11" customWidth="1"/>
-    <col min="15" max="15" width="46.109375" style="9" customWidth="1"/>
-    <col min="16" max="16" width="10.88671875" style="9" customWidth="1"/>
-    <col min="17" max="17" width="21.88671875" style="9" customWidth="1"/>
-    <col min="18" max="18" width="86.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="50.88671875" style="11" customWidth="1"/>
-    <col min="20" max="250" width="11.44140625" style="9" customWidth="1"/>
-    <col min="251" max="251" width="9.109375" style="9" customWidth="1"/>
-    <col min="252" max="16384" width="9.109375" style="9"/>
+    <col min="11" max="11" width="12.5703125" style="9" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" style="9" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" style="39" customWidth="1"/>
+    <col min="14" max="14" width="21.85546875" style="11" customWidth="1"/>
+    <col min="15" max="15" width="46.140625" style="9" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" style="9" customWidth="1"/>
+    <col min="17" max="17" width="21.85546875" style="9" customWidth="1"/>
+    <col min="18" max="18" width="86.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="50.85546875" style="11" customWidth="1"/>
+    <col min="20" max="250" width="11.42578125" style="9" customWidth="1"/>
+    <col min="251" max="251" width="9.140625" style="9" customWidth="1"/>
+    <col min="252" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1124,7 +1124,7 @@
       <c r="N1" s="10"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
@@ -1143,12 +1143,12 @@
       <c r="N2" s="14"/>
       <c r="O2" s="15"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -1164,12 +1164,12 @@
       <c r="N3" s="14"/>
       <c r="O3" s="15"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>6</v>
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
@@ -1186,12 +1186,12 @@
       <c r="O4" s="15"/>
       <c r="P4" s="16"/>
       <c r="Q4" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" s="17" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>8</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="18"/>
@@ -1209,12 +1209,12 @@
       <c r="O5" s="20"/>
       <c r="P5" s="21"/>
       <c r="Q5" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" s="50" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="50" t="s">
-        <v>10</v>
       </c>
       <c r="B6" s="51"/>
       <c r="C6" s="51"/>
@@ -1231,9 +1231,9 @@
       <c r="N6" s="51"/>
       <c r="O6" s="52"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="57" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="55"/>
       <c r="C7" s="55"/>
@@ -1250,9 +1250,9 @@
       <c r="N7" s="55"/>
       <c r="O7" s="56"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="54" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="55"/>
       <c r="C8" s="55"/>
@@ -1269,13 +1269,13 @@
       <c r="N8" s="55"/>
       <c r="O8" s="56"/>
     </row>
-    <row r="9" spans="1:19" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="27"/>
       <c r="D9" s="53" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" s="51"/>
       <c r="F9" s="52"/>
@@ -1286,93 +1286,93 @@
       <c r="K9" s="42"/>
       <c r="L9" s="42"/>
       <c r="N9" s="46" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O9" s="22"/>
     </row>
-    <row r="10" spans="1:19" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:19" ht="23.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="40"/>
       <c r="C10" s="45"/>
       <c r="D10" s="47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" s="48"/>
       <c r="F10" s="49"/>
       <c r="G10" s="60" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H10" s="48"/>
       <c r="I10" s="49"/>
       <c r="J10" s="59" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K10" s="48"/>
       <c r="L10" s="49"/>
       <c r="N10" s="41"/>
       <c r="O10" s="22"/>
     </row>
-    <row r="11" spans="1:19" s="11" customFormat="1" ht="52.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" s="11" customFormat="1" ht="52.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="C11" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="D11" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="E11" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="F11" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="31" t="s">
+      <c r="G11" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="M11" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="I11" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="K11" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="L11" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="M11" s="32" t="s">
+      <c r="N11" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="N11" s="32" t="s">
+      <c r="O11" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="O11" s="29" t="s">
+      <c r="P11" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="P11" s="33" t="s">
+      <c r="Q11" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="Q11" s="33" t="s">
+      <c r="R11" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="R11" s="33" t="s">
+      <c r="S11" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="S11" s="34" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="23">
         <v>6</v>
@@ -1382,24 +1382,24 @@
       <c r="E12" s="24"/>
       <c r="F12" s="24"/>
       <c r="G12" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H12" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I12" s="24"/>
       <c r="J12" s="24"/>
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N12" s="25"/>
       <c r="O12" s="35"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="23">
         <v>10</v>
@@ -1410,23 +1410,23 @@
       <c r="F13" s="24"/>
       <c r="G13" s="24"/>
       <c r="H13" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J13" s="24"/>
       <c r="K13" s="24"/>
       <c r="L13" s="24"/>
       <c r="M13" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N13" s="25"/>
       <c r="O13" s="35"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="23">
         <v>100</v>
@@ -1436,7 +1436,7 @@
       <c r="E14" s="24"/>
       <c r="F14" s="24"/>
       <c r="G14" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H14" s="24"/>
       <c r="I14" s="24"/>
@@ -1444,14 +1444,14 @@
       <c r="K14" s="24"/>
       <c r="L14" s="24"/>
       <c r="M14" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N14" s="25"/>
       <c r="O14" s="35"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="23">
         <v>9</v>
@@ -1467,14 +1467,14 @@
       <c r="K15" s="24"/>
       <c r="L15" s="24"/>
       <c r="M15" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N15" s="25"/>
       <c r="O15" s="35"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="23">
         <v>87</v>
@@ -1484,24 +1484,24 @@
       <c r="E16" s="24"/>
       <c r="F16" s="24"/>
       <c r="G16" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I16" s="24"/>
       <c r="J16" s="24"/>
       <c r="K16" s="24"/>
       <c r="L16" s="24"/>
       <c r="M16" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N16" s="25"/>
       <c r="O16" s="35"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="23">
         <v>56</v>
@@ -1513,20 +1513,20 @@
       <c r="G17" s="24"/>
       <c r="H17" s="24"/>
       <c r="I17" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J17" s="24"/>
       <c r="K17" s="24"/>
       <c r="L17" s="24"/>
       <c r="M17" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N17" s="25"/>
       <c r="O17" s="35"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="23">
         <v>32</v>
@@ -1536,24 +1536,24 @@
       <c r="E18" s="24"/>
       <c r="F18" s="24"/>
       <c r="G18" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H18" s="24"/>
       <c r="I18" s="24"/>
       <c r="J18" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K18" s="24"/>
       <c r="L18" s="24"/>
       <c r="M18" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N18" s="25"/>
       <c r="O18" s="35"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" s="23">
         <v>78</v>
@@ -1564,51 +1564,51 @@
       <c r="F19" s="24"/>
       <c r="G19" s="24"/>
       <c r="H19" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J19" s="24"/>
       <c r="K19" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L19" s="24"/>
       <c r="M19" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N19" s="25"/>
       <c r="O19" s="35"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="23">
         <v>123456</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="24"/>
       <c r="F20" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I20" s="24"/>
       <c r="J20" s="24"/>
       <c r="K20" s="24"/>
       <c r="L20" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M20" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N20" s="25"/>
       <c r="O20" s="35"/>
@@ -1616,41 +1616,41 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="23" t="s">
-        <v>38</v>
-      </c>
       <c r="C21" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D21" s="24"/>
       <c r="E21" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F21" s="24"/>
       <c r="G21" s="24"/>
       <c r="H21" s="24"/>
       <c r="I21" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J21" s="24"/>
       <c r="K21" s="24"/>
       <c r="L21" s="24"/>
       <c r="M21" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N21" s="25"/>
       <c r="O21" s="35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P21" s="9">
         <v>7</v>
       </c>
       <c r="Q21" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R21" s="9">
         <v>8</v>
@@ -1659,45 +1659,45 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="23" t="s">
-        <v>40</v>
-      </c>
       <c r="C22" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D22" s="24"/>
       <c r="E22" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G22" s="24"/>
       <c r="H22" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I22" s="24"/>
       <c r="J22" s="24"/>
       <c r="K22" s="24"/>
       <c r="L22" s="24"/>
       <c r="M22" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N22" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O22" s="35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P22" s="9">
         <v>6</v>
       </c>
       <c r="Q22" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R22" s="9">
         <v>7</v>
@@ -1706,49 +1706,49 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="23" t="s">
-        <v>42</v>
-      </c>
       <c r="C23" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F23" s="24"/>
       <c r="G23" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H23" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J23" s="24"/>
       <c r="K23" s="24"/>
       <c r="L23" s="24"/>
       <c r="M23" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N23" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O23" s="35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P23" s="9">
         <v>5</v>
       </c>
       <c r="Q23" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R23" s="9">
         <v>6</v>
@@ -1757,45 +1757,45 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="23" t="s">
-        <v>44</v>
-      </c>
       <c r="C24" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E24" s="24"/>
       <c r="F24" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G24" s="24"/>
       <c r="H24" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I24" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J24" s="24"/>
       <c r="K24" s="24"/>
       <c r="L24" s="24"/>
       <c r="M24" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N24" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O24" s="35"/>
       <c r="P24" s="9">
         <v>10</v>
       </c>
       <c r="Q24" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R24" s="9">
         <v>5</v>
@@ -1804,23 +1804,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="23" t="s">
-        <v>44</v>
-      </c>
       <c r="C25" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D25" s="24"/>
       <c r="E25" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F25" s="24"/>
       <c r="G25" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H25" s="24"/>
       <c r="I25" s="24"/>
@@ -1828,19 +1828,19 @@
       <c r="K25" s="24"/>
       <c r="L25" s="24"/>
       <c r="M25" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="N25" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="N25" s="25" t="s">
-        <v>64</v>
-      </c>
       <c r="O25" s="35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P25" s="9">
         <v>6</v>
       </c>
       <c r="Q25" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R25" s="9">
         <v>4</v>
@@ -1891,276 +1891,276 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
     <col min="4" max="4" width="60" customWidth="1"/>
-    <col min="5" max="256" width="11.44140625" customWidth="1"/>
+    <col min="5" max="256" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>

</xml_diff>